<commit_message>
feat: excel and queries,medium proyect
</commit_message>
<xml_diff>
--- a/Sistema/data/equipos.xlsx
+++ b/Sistema/data/equipos.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Prestado</t>
+          <t>Disponible</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -519,7 +519,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t>Prestado</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Prestado</t>
+          <t>Disponible</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -588,7 +588,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t>Prestado</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t>Prestado</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Prestado</t>
+          <t>Disponible</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">

</xml_diff>

<commit_message>
feat:report pdf/excel completed, more register
</commit_message>
<xml_diff>
--- a/Sistema/data/equipos.xlsx
+++ b/Sistema/data/equipos.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t>Prestado</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t>Prestado</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t>Prestado</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t>Prestado</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -680,7 +680,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Disponible</t>
+          <t>Prestado</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">

</xml_diff>